<commit_message>
AP-3549 AP-3574 Various improvements in CSV Importer (#892)
* AP-3549 Replace logic to detect different types of separators in Log importer

* Bug fix

* Fix unit tests

* Clean up

* AP-3574 Avoid trimming when process headers.

* Code formatting
</commit_message>
<xml_diff>
--- a/Apromore-Custom-Plugins/CSVImporter-Logic/src/test/resources/test10-eventAttribute.xlsx
+++ b/Apromore-Custom-Plugins/CSVImporter-Logic/src/test/resources/test10-eventAttribute.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24004"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/own_strong/Dev/Apromore-prod/ApromoreEE/ApromoreCore/Apromore-Custom-Plugins/CSVImporter-Logic/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FEDF108-1E60-7F42-A026-ED4B8ABAAFBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{45A073C4-09BE-426D-BA10-E9A68B34D4DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test10-eventAttribute" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
   <si>
     <t>case id</t>
   </si>
@@ -34,6 +45,9 @@
     <t>completion time</t>
   </si>
   <si>
+    <t>process type</t>
+  </si>
+  <si>
     <t>case2</t>
   </si>
   <si>
@@ -56,16 +70,13 @@
   </si>
   <si>
     <t>2019-09-23T15:13:05.133</t>
-  </si>
-  <si>
-    <t>process type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -899,15 +910,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -921,57 +932,108 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4">
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7">
         <v>1</v>
       </c>
     </row>

</xml_diff>